<commit_message>
KDE and heatmap Mark
</commit_message>
<xml_diff>
--- a/EAIAK/Helixvstemperature.xlsx
+++ b/EAIAK/Helixvstemperature.xlsx
@@ -193,7 +193,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -260,7 +260,7 @@
                     <c:v/>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v/>
+                    <c:v>0.0680038106571</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v/>
@@ -290,7 +290,7 @@
                     <c:v/>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v/>
+                    <c:v>0.0680038106571</c:v>
                   </c:pt>
                   <c:pt idx="3">
                     <c:v/>
@@ -351,7 +351,7 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v/>
+                  <c:v>0.568725</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v/>
@@ -402,6 +402,7 @@
             </c:spPr>
           </c:marker>
           <c:dLbls>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -471,11 +472,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="60780695"/>
-        <c:axId val="7476022"/>
+        <c:axId val="5045583"/>
+        <c:axId val="71846341"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="60780695"/>
+        <c:axId val="5045583"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -510,12 +511,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="7476022"/>
+        <c:crossAx val="71846341"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="7476022"/>
+        <c:axId val="71846341"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -559,7 +560,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="60780695"/>
+        <c:crossAx val="5045583"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -597,9 +598,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>157320</xdr:colOff>
+      <xdr:colOff>156960</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>38160</xdr:rowOff>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -607,8 +608,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3553920" y="57240"/>
-        <a:ext cx="5004360" cy="3719520"/>
+        <a:off x="3506400" y="57240"/>
+        <a:ext cx="4917960" cy="3719160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -629,12 +630,12 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N32" activeCellId="0" sqref="N32"/>
+      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -694,8 +695,12 @@
       <c r="C4" s="1" t="n">
         <v>0.0876410149416</v>
       </c>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
+      <c r="D4" s="0" t="n">
+        <v>0.568725</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>0.0680038106571</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">

</xml_diff>

<commit_message>
added EAIAK 150 Mark
</commit_message>
<xml_diff>
--- a/EAIAK/Helixvstemperature.xlsx
+++ b/EAIAK/Helixvstemperature.xlsx
@@ -193,7 +193,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -272,7 +272,7 @@
                     <c:v/>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v/>
+                    <c:v>0.0375345609258</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v/>
@@ -305,7 +305,7 @@
                     <c:v/>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v/>
+                    <c:v>0.0375345609258</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v/>
@@ -372,7 +372,7 @@
                   <c:v/>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>0.0873083333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v/>
@@ -490,11 +490,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="27013545"/>
-        <c:axId val="45778686"/>
+        <c:axId val="94172096"/>
+        <c:axId val="11596368"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="27013545"/>
+        <c:axId val="94172096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -529,12 +529,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="45778686"/>
+        <c:crossAx val="11596368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="45778686"/>
+        <c:axId val="11596368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -578,7 +578,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27013545"/>
+        <c:crossAx val="94172096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -616,9 +616,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>156600</xdr:colOff>
+      <xdr:colOff>156240</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>37440</xdr:rowOff>
+      <xdr:rowOff>37080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -626,8 +626,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3458880" y="57240"/>
-        <a:ext cx="4831920" cy="3881520"/>
+        <a:off x="3411360" y="57240"/>
+        <a:ext cx="4745880" cy="3881160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -648,13 +648,10 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
-  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -779,8 +776,12 @@
       <c r="C8" s="1" t="n">
         <v>0.0577740804773</v>
       </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
+      <c r="D8" s="0" t="n">
+        <v>0.0873083333333</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.0375345609258</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">

</xml_diff>

<commit_message>
added 125 EAIAK Mark
</commit_message>
<xml_diff>
--- a/EAIAK/Helixvstemperature.xlsx
+++ b/EAIAK/Helixvstemperature.xlsx
@@ -272,7 +272,7 @@
                     <c:v>0.148169325061</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v/>
+                    <c:v>0.0547983823514</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>0.0375345609258</c:v>
@@ -308,7 +308,7 @@
                     <c:v>0.148169325061</c:v>
                   </c:pt>
                   <c:pt idx="6">
-                    <c:v/>
+                    <c:v>0.0547983823514</c:v>
                   </c:pt>
                   <c:pt idx="7">
                     <c:v>0.0375345609258</c:v>
@@ -381,7 +381,7 @@
                   <c:v>0.308833333333</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v/>
+                  <c:v>0.0862583333333</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0873083333333</c:v>
@@ -508,11 +508,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="41281374"/>
-        <c:axId val="30189720"/>
+        <c:axId val="89428424"/>
+        <c:axId val="84602886"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41281374"/>
+        <c:axId val="89428424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -547,12 +547,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="30189720"/>
+        <c:crossAx val="84602886"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="30189720"/>
+        <c:axId val="84602886"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -596,7 +596,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="41281374"/>
+        <c:crossAx val="89428424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -634,9 +634,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>154800</xdr:colOff>
+      <xdr:colOff>154440</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>36000</xdr:rowOff>
+      <xdr:rowOff>35640</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -644,8 +644,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="3411720" y="57240"/>
-        <a:ext cx="4744080" cy="4042440"/>
+        <a:off x="3554640" y="57240"/>
+        <a:ext cx="5000760" cy="4042080"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -666,10 +666,13 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
+      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.50510204081633"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -799,6 +802,12 @@
       </c>
       <c r="C8" s="0" t="n">
         <v>0.0683777695966</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>0.0862583333333</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0.0547983823514</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>